<commit_message>
Added new recording for segment A
</commit_message>
<xml_diff>
--- a/MyFrankCrum_EMP/Segment_A.xlsx
+++ b/MyFrankCrum_EMP/Segment_A.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MFC_Ranorex\MyFrankCrum_EMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA2DBF-A076-4D56-8FE9-6AE1D42BB37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCD968F-5167-42E6-AEF4-EA2DC7090D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{9ADB6619-802A-418E-A83B-66F8F437DA2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{9ADB6619-802A-418E-A83B-66F8F437DA2E}"/>
   </bookViews>
   <sheets>
     <sheet name="TC's_Sheet" sheetId="1" r:id="rId1"/>
     <sheet name="Common_Data" sheetId="2" r:id="rId2"/>
     <sheet name="WSE_Login_Page" sheetId="3" r:id="rId3"/>
-    <sheet name="ER_Login_Page" sheetId="8" r:id="rId4"/>
-    <sheet name="WSE_Home_Page" sheetId="4" r:id="rId5"/>
-    <sheet name="Current_Paycheck" sheetId="5" r:id="rId6"/>
-    <sheet name="Paycheck_History" sheetId="6" r:id="rId7"/>
-    <sheet name="Direct_Deposit_Settings" sheetId="7" r:id="rId8"/>
+    <sheet name="WSE_Home_Page" sheetId="4" r:id="rId4"/>
+    <sheet name="Current_Paycheck" sheetId="5" r:id="rId5"/>
+    <sheet name="Paycheck_History" sheetId="6" r:id="rId6"/>
+    <sheet name="Direct_Deposit_Settings" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>TC's ID</t>
   </si>
@@ -137,6 +136,9 @@
   </si>
   <si>
     <t>mfcdev02.frankcrum.com</t>
+  </si>
+  <si>
+    <t>ER_W_2s</t>
   </si>
 </sst>
 </file>
@@ -520,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13632003-B44A-473E-809C-BEC97166C5CC}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +600,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>8101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" location="WSE_Login_Page!A1" display="WSE_Login_Page" xr:uid="{8A9213C9-1A75-4FDC-B0B8-A008129BB639}"/>
@@ -605,6 +618,7 @@
     <hyperlink ref="C4" location="Current_Paycheck!A1" display="Current_Paycheck" xr:uid="{BB32D9EB-0858-4C9F-A817-79693B70EE9F}"/>
     <hyperlink ref="C5" location="Paycheck_History!A1" display="Paycheck_History" xr:uid="{09401BCA-FC0D-42B9-BBC6-401BC6E37CB7}"/>
     <hyperlink ref="C6" location="Direct_Deposit_Settings!A1" display="Direct_Deposit_Settings" xr:uid="{C448DC7A-CC82-421E-AF01-E0945571BF4A}"/>
+    <hyperlink ref="C7" location="ER_W_2s!A1" display="ER_W_2s" xr:uid="{9E988C09-4EAB-441B-9262-BCE70B1693B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -614,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD85CB5E-9145-4B3C-8387-A5E2F209FA67}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -717,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD931B9-2358-492E-80F5-E4F2BF0FAC33}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,73 +863,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB59DE2-ED84-4FE2-B74D-56B01BE3A218}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" t="str">
-        <f>Common_Data!A2</f>
-        <v>Chrome</v>
-      </c>
-      <c r="D2" t="str">
-        <f>Common_Data!B2</f>
-        <v>https://mfcqa01.frankcrum.com</v>
-      </c>
-      <c r="E2" t="str">
-        <f>Common_Data!C2</f>
-        <v>mfcqa01.frankcrum.com</v>
-      </c>
-      <c r="F2" t="str">
-        <f>Common_Data!D2</f>
-        <v>JMartin123</v>
-      </c>
-      <c r="G2" t="str">
-        <f>Common_Data!E2</f>
-        <v>JMartin123$</v>
-      </c>
-      <c r="H2" t="str">
-        <f>Common_Data!F2</f>
-        <v>Lucky Dog</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69516588-FCB8-4C90-B6EA-2A9B02107921}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -1053,7 +1000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A34D7F-273D-4EE9-BD08-7B331B23E0F9}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1128,7 +1075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{151CAC0C-0656-42A5-85A7-9958B233F3BB}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1203,7 +1150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79FCDEF-0DAE-401B-A69A-B768F50E3B6B}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>